<commit_message>
Changes in ECO file
Changes in ECO file
</commit_message>
<xml_diff>
--- a/SR Smart App/ECO_SRSMART_ANDROID_01.01.11.xlsx
+++ b/SR Smart App/ECO_SRSMART_ANDROID_01.01.11.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560"/>
+    <workbookView xWindow="200" yWindow="940" windowWidth="25600" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="ECO FORM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t xml:space="preserve">ECO # </t>
   </si>
@@ -130,15 +130,6 @@
   </si>
   <si>
     <t>Jul 07, 2015</t>
-  </si>
-  <si>
-    <t>BY: QA Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">By: </t>
   </si>
   <si>
     <t>Software Engineering</t>
@@ -161,6 +152,18 @@
   <si>
     <t xml:space="preserve">RELEASENOTE_SRSMART_ANDROID_01.01.11.docx  - https://github.com/DelphianSystems/SecuRemote/tree/master/SR%20Smart%20App
 </t>
+  </si>
+  <si>
+    <t>By:  Paresh Vaghela</t>
+  </si>
+  <si>
+    <t>By: Paresh Vaghela</t>
+  </si>
+  <si>
+    <t>BY: Pavan</t>
+  </si>
+  <si>
+    <t>Date: 21/07/15</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -517,8 +520,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -647,6 +659,66 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -689,71 +761,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2000,8 +2018,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>175846</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2932,8 +2950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2982,142 +3000,142 @@
       <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="62"/>
+      <c r="F3" s="46"/>
       <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15" customHeight="1">
       <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
+      <c r="C4" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
     </row>
     <row r="5" spans="2:8" ht="28" customHeight="1">
       <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="C5" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="73"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="75"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
     </row>
     <row r="9" spans="2:8" ht="38" customHeight="1">
       <c r="B9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
+      <c r="C9" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="60"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="60"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="62"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>13</v>
@@ -3132,112 +3150,112 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58" t="s">
+      <c r="D17" s="61"/>
+      <c r="E17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="58"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="54"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="74"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="54"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="74"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="55"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="57"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="77"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="9" t="s">
@@ -3303,13 +3321,13 @@
       <c r="C31" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="45"/>
-      <c r="F31" s="46"/>
+      <c r="D31" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="5" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="H31" s="8"/>
     </row>
@@ -3318,11 +3336,11 @@
       <c r="C32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="46"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>1</v>
       </c>
@@ -3333,13 +3351,13 @@
         <v>30</v>
       </c>
       <c r="C33" s="23"/>
-      <c r="D33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="45"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="5" t="s">
-        <v>1</v>
+      <c r="D33" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="65"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="44" t="s">
+        <v>47</v>
       </c>
       <c r="H33" s="8"/>
     </row>
@@ -3359,12 +3377,12 @@
       <c r="C35" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="48"/>
+      <c r="D35" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="68"/>
       <c r="F35" s="27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G35" s="27" t="s">
         <v>33</v>
@@ -3396,7 +3414,7 @@
         <v>35</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D38" s="28"/>
       <c r="E38" s="34"/>
@@ -3508,32 +3526,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B22:H25"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:H21"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B22:H25"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="C7:H7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1" display="RELEASENOTE_SRSMART_ANDROID_01.01.10.docx  - https://github.com/DelphianSystems/SecuRemote/tree/master/SR%20Smart%20App_x000d_"/>

</xml_diff>